<commit_message>
preparing for a coilcube purchase
</commit_message>
<xml_diff>
--- a/coilcube/rev_c/coilcube_bom.xlsx
+++ b/coilcube/rev_c/coilcube_bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="93">
   <si>
     <t>Qty</t>
   </si>
@@ -38,6 +38,9 @@
     <t>DIGIKEY</t>
   </si>
   <si>
+    <t>DIGIREEL</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
     <t>445-1316-1-ND</t>
   </si>
   <si>
+    <t>445-1316-6-ND</t>
+  </si>
+  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -68,6 +74,9 @@
     <t>445-1321-1-ND</t>
   </si>
   <si>
+    <t>445-1321-6-ND</t>
+  </si>
+  <si>
     <t>2.2uF</t>
   </si>
   <si>
@@ -92,6 +101,9 @@
     <t>445-5178-1-ND</t>
   </si>
   <si>
+    <t>445-5178-6-ND</t>
+  </si>
+  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -107,6 +119,9 @@
     <t>399-8152-1-ND</t>
   </si>
   <si>
+    <t>399-8152-6-ND</t>
+  </si>
+  <si>
     <t>47uF</t>
   </si>
   <si>
@@ -125,6 +140,9 @@
     <t>399-3700-1-ND</t>
   </si>
   <si>
+    <t>399-3700-6-ND</t>
+  </si>
+  <si>
     <t>100uF 25V</t>
   </si>
   <si>
@@ -137,6 +155,9 @@
     <t>399-5175-1-ND</t>
   </si>
   <si>
+    <t>399-5175-6-ND</t>
+  </si>
+  <si>
     <t>SCREW-TERMINAL_2_0.100</t>
   </si>
   <si>
@@ -167,6 +188,9 @@
     <t>587-1625-1-ND</t>
   </si>
   <si>
+    <t>587-1625-6-ND</t>
+  </si>
+  <si>
     <t>4.7k</t>
   </si>
   <si>
@@ -185,6 +209,9 @@
     <t>P4.7KGCT-ND</t>
   </si>
   <si>
+    <t>P4.7KGDKR-ND</t>
+  </si>
+  <si>
     <t>1M</t>
   </si>
   <si>
@@ -194,6 +221,9 @@
     <t>RHM1.00MCFCT-ND</t>
   </si>
   <si>
+    <t>RHM1.00MCFDKR-ND</t>
+  </si>
+  <si>
     <t>4.7M</t>
   </si>
   <si>
@@ -203,6 +233,9 @@
     <t>RHM4.7MCGCT-ND</t>
   </si>
   <si>
+    <t>RHM4.7MCGDKR-ND</t>
+  </si>
+  <si>
     <t>NCHAN_MOSFET</t>
   </si>
   <si>
@@ -212,10 +245,16 @@
     <t>SI1302DL-T1-GE3CT-ND</t>
   </si>
   <si>
+    <t>SI1302DL-T1-GE3DKR-ND</t>
+  </si>
+  <si>
     <t>T3</t>
   </si>
   <si>
     <t>568-3244-1-ND</t>
+  </si>
+  <si>
+    <t>568-3244-6-ND</t>
   </si>
   <si>
     <t>EPIC-CORE_A</t>
@@ -359,13 +398,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F13" activeCellId="0" pane="topLeft" sqref="F13"/>
+      <selection activeCell="G11" activeCellId="0" pane="topLeft" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.47959183673469"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.3265306122449"/>
@@ -373,8 +412,9 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.9948979591837"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.1071428571429"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.2448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.1326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.7295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="61.1326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -402,28 +442,34 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
@@ -431,22 +477,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
@@ -454,19 +503,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
@@ -474,22 +523,25 @@
         <v>1</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
@@ -497,22 +549,25 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
@@ -520,22 +575,25 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
@@ -543,19 +601,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
@@ -563,22 +624,22 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
@@ -586,22 +647,25 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1210</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
@@ -609,22 +673,25 @@
         <v>3</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
@@ -632,22 +699,25 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
@@ -655,22 +725,25 @@
         <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="D13" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>61</v>
+        <v>71</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
@@ -678,19 +751,22 @@
         <v>2</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>64</v>
+        <v>75</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
@@ -698,19 +774,22 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>66</v>
+        <v>78</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
@@ -718,19 +797,19 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>70</v>
+        <v>82</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
@@ -738,22 +817,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
@@ -761,19 +840,19 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>